<commit_message>
Forgot to have prices
</commit_message>
<xml_diff>
--- a/Vendors.xlsx
+++ b/Vendors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Catherine-Schiber-P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E44E16B-0199-463D-AEDE-3E1E3A08519E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98392C1E-245F-4C57-A333-8A772A952016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1720" yWindow="2890" windowWidth="16800" windowHeight="9670" activeTab="1" xr2:uid="{BAF409F4-9796-4393-8D4C-DBA9A41D9979}"/>
+    <workbookView xWindow="1720" yWindow="2890" windowWidth="16800" windowHeight="9670" activeTab="2" xr2:uid="{BAF409F4-9796-4393-8D4C-DBA9A41D9979}"/>
   </bookViews>
   <sheets>
     <sheet name="Grocery" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>Item</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>Lotion</t>
+  </si>
+  <si>
+    <t>Price</t>
   </si>
 </sst>
 </file>
@@ -440,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBD4118-67C7-48E3-BFF0-6775087DB63C}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -451,68 +454,92 @@
     <col min="1" max="1" width="14.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2">
+        <v>11.99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C5">
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>14</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>15</v>
       </c>
       <c r="B7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C7">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
       <c r="B8">
         <v>5</v>
+      </c>
+      <c r="C8">
+        <v>6.5</v>
       </c>
     </row>
   </sheetData>
@@ -522,10 +549,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6C95482-DE57-46FD-9C11-5E839098DF48}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -533,44 +560,59 @@
     <col min="1" max="1" width="18.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2">
+        <v>4.99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3">
+        <v>11.99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4">
+        <v>11.99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5">
         <v>5</v>
+      </c>
+      <c r="C5">
+        <v>9.99</v>
       </c>
     </row>
   </sheetData>
@@ -580,10 +622,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A27E41A-BC4E-4F02-84E6-D0EB8F4E5410}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -591,52 +633,70 @@
     <col min="1" max="1" width="19.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
         <v>2</v>
+      </c>
+      <c r="C6">
+        <v>12.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>